<commit_message>
add species longevity info and norm_age to data set
</commit_message>
<xml_diff>
--- a/data/species.xlsx
+++ b/data/species.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuel_bohn/Work/Cloud/ManyPrimates/git/mp1_short_term_memory/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96064B37-187B-8A4A-A68F-DE53BC3B4D16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C261BFE-30DA-FD46-8039-6EB9CBA06F39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-1240" windowWidth="38400" windowHeight="21140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -375,7 +375,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{0B4DAEC2-C34A-0347-87C5-66B3072A6096}" name="species_data" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/manuel_bohn/Work/Cloud/ManyPrimates/git/mp1_short_term_memory/data/species_data.csv" decimal="," thousands="." comma="1">
+    <textPr sourceFile="/Users/manuel_bohn/Work/Cloud/ManyPrimates/git/mp1_short_term_memory/data/species_data.csv" decimal="," thousands="." comma="1">
       <textFields count="8">
         <textField/>
         <textField/>
@@ -389,7 +389,7 @@
     </textPr>
   </connection>
   <connection id="2" xr16:uid="{FC8F7AB8-3250-F844-9327-9C7E5BCE3306}" name="species_data1" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/manuel_bohn/Work/Cloud/ManyPrimates/git/mp1_short_term_memory/data/species_data.csv" decimal="," thousands="." comma="1">
+    <textPr sourceFile="/Users/manuel_bohn/Work/Cloud/ManyPrimates/git/mp1_short_term_memory/data/species_data.csv" decimal="," thousands="." comma="1">
       <textFields count="8">
         <textField/>
         <textField/>
@@ -406,7 +406,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2065" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2075" uniqueCount="341">
   <si>
     <t>Species_English</t>
   </si>
@@ -1647,6 +1647,27 @@
   </si>
   <si>
     <t>29.5</t>
+  </si>
+  <si>
+    <t>26.75</t>
+  </si>
+  <si>
+    <t>30.5</t>
+  </si>
+  <si>
+    <t>17.9</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Longevity of mammals in captivity; from the living collections of the world." by Richard Weigl (Kleine Senckenberg-Reihe 48, 2005)</t>
+  </si>
+  <si>
+    <t>Data from C. chiropotes</t>
+  </si>
+  <si>
+    <t>Data from Eulemur macaco</t>
   </si>
 </sst>
 </file>
@@ -1922,14 +1943,14 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2188,7 +2209,7 @@
       <c r="E1" t="s">
         <v>273</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="45" t="s">
         <v>274</v>
       </c>
       <c r="G1" t="s">
@@ -2214,7 +2235,7 @@
       <c r="E2" t="s">
         <v>278</v>
       </c>
-      <c r="F2" s="47" t="s">
+      <c r="F2" s="45" t="s">
         <v>279</v>
       </c>
       <c r="G2">
@@ -2240,7 +2261,7 @@
       <c r="E3" t="s">
         <v>278</v>
       </c>
-      <c r="F3" s="47" t="s">
+      <c r="F3" s="45" t="s">
         <v>282</v>
       </c>
       <c r="G3">
@@ -2266,7 +2287,7 @@
       <c r="E4" t="s">
         <v>285</v>
       </c>
-      <c r="F4" s="47" t="s">
+      <c r="F4" s="45" t="s">
         <v>306</v>
       </c>
       <c r="G4">
@@ -2292,7 +2313,7 @@
       <c r="E5" t="s">
         <v>285</v>
       </c>
-      <c r="F5" s="47" t="s">
+      <c r="F5" s="45" t="s">
         <v>306</v>
       </c>
       <c r="G5">
@@ -2315,7 +2336,7 @@
       <c r="E6" t="s">
         <v>285</v>
       </c>
-      <c r="F6" s="47" t="s">
+      <c r="F6" s="45" t="s">
         <v>289</v>
       </c>
       <c r="G6">
@@ -2341,7 +2362,7 @@
       <c r="E7" t="s">
         <v>291</v>
       </c>
-      <c r="F7" s="47" t="s">
+      <c r="F7" s="45" t="s">
         <v>307</v>
       </c>
       <c r="G7">
@@ -2367,7 +2388,7 @@
       <c r="E8" t="s">
         <v>291</v>
       </c>
-      <c r="F8" s="47" t="s">
+      <c r="F8" s="45" t="s">
         <v>308</v>
       </c>
       <c r="G8">
@@ -2393,7 +2414,7 @@
       <c r="E9" t="s">
         <v>291</v>
       </c>
-      <c r="F9" s="47" t="s">
+      <c r="F9" s="45" t="s">
         <v>309</v>
       </c>
       <c r="G9">
@@ -2419,7 +2440,7 @@
       <c r="E10" t="s">
         <v>296</v>
       </c>
-      <c r="F10" s="47" t="s">
+      <c r="F10" s="45" t="s">
         <v>297</v>
       </c>
       <c r="G10">
@@ -2445,7 +2466,7 @@
       <c r="E11" t="s">
         <v>296</v>
       </c>
-      <c r="F11" s="47" t="s">
+      <c r="F11" s="45" t="s">
         <v>310</v>
       </c>
       <c r="G11">
@@ -2471,7 +2492,7 @@
       <c r="E12" t="s">
         <v>296</v>
       </c>
-      <c r="F12" s="47" t="s">
+      <c r="F12" s="45" t="s">
         <v>302</v>
       </c>
       <c r="G12">
@@ -2497,7 +2518,7 @@
       <c r="E13" t="s">
         <v>296</v>
       </c>
-      <c r="F13" s="47" t="s">
+      <c r="F13" s="45" t="s">
         <v>311</v>
       </c>
       <c r="G13">
@@ -2874,7 +2895,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>51</v>
       </c>
@@ -2988,7 +3009,7 @@
         <v>2110</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>57</v>
       </c>
@@ -3051,7 +3072,7 @@
         <v>38.5</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>60</v>
       </c>
@@ -3167,7 +3188,7 @@
         <v>1755</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>63</v>
       </c>
@@ -3286,7 +3307,7 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>69</v>
       </c>
@@ -3387,7 +3408,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>71</v>
       </c>
@@ -3465,7 +3486,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>73</v>
       </c>
@@ -3594,7 +3615,7 @@
         <v>3650</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>77</v>
       </c>
@@ -3712,7 +3733,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>79</v>
       </c>
@@ -3818,7 +3839,7 @@
         <v>860.8</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>81</v>
       </c>
@@ -3888,7 +3909,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>83</v>
       </c>
@@ -3973,7 +3994,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>86</v>
       </c>
@@ -4045,7 +4066,7 @@
         <v>3.35</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>88</v>
       </c>
@@ -4113,7 +4134,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>91</v>
       </c>
@@ -4190,7 +4211,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>93</v>
       </c>
@@ -4294,7 +4315,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>95</v>
       </c>
@@ -4415,7 +4436,7 @@
         <v>549.79999999999995</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>97</v>
       </c>
@@ -4564,7 +4585,7 @@
         <v>14.9</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>101</v>
       </c>
@@ -4626,7 +4647,7 @@
         <v>3.49</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>103</v>
       </c>
@@ -4713,7 +4734,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>105</v>
       </c>
@@ -4775,7 +4796,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>107</v>
       </c>
@@ -4904,7 +4925,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>111</v>
       </c>
@@ -4983,7 +5004,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>113</v>
       </c>
@@ -5077,7 +5098,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
         <v>115</v>
       </c>
@@ -5152,7 +5173,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>117</v>
       </c>
@@ -5253,7 +5274,7 @@
         <v>598.79999999999995</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>119</v>
       </c>
@@ -5324,7 +5345,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>121</v>
       </c>
@@ -5405,7 +5426,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>123</v>
       </c>
@@ -5505,7 +5526,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>127</v>
       </c>
@@ -5658,7 +5679,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>131</v>
       </c>
@@ -5733,7 +5754,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
         <v>133</v>
       </c>
@@ -5838,7 +5859,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>135</v>
       </c>
@@ -5912,7 +5933,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
         <v>137</v>
       </c>
@@ -5983,7 +6004,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
         <v>139</v>
       </c>
@@ -6076,7 +6097,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
         <v>141</v>
       </c>
@@ -6158,7 +6179,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
         <v>143</v>
       </c>
@@ -6220,7 +6241,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="s">
         <v>145</v>
       </c>
@@ -6352,7 +6373,7 @@
         <v>21.41</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
         <v>150</v>
       </c>
@@ -6418,7 +6439,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:39" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>152</v>
       </c>
@@ -12718,7 +12739,7 @@
       <c r="E2" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="48" t="s">
         <v>170</v>
       </c>
       <c r="G2" s="33" t="s">
@@ -12830,7 +12851,7 @@
       <c r="E3" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="45"/>
+      <c r="F3" s="49"/>
       <c r="G3" s="34" t="s">
         <v>182</v>
       </c>
@@ -12923,7 +12944,7 @@
       <c r="E4" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="F4" s="45"/>
+      <c r="F4" s="49"/>
       <c r="G4" s="33" t="s">
         <v>45</v>
       </c>
@@ -13028,7 +13049,7 @@
       <c r="E5" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="45"/>
+      <c r="F5" s="49"/>
       <c r="G5" s="33" t="s">
         <v>45</v>
       </c>
@@ -19448,7 +19469,7 @@
   <dimension ref="A1:Z55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E46"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -19471,8 +19492,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="44" t="s">
         <v>305</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -19488,7 +19512,7 @@
       <c r="D2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="49" t="s">
+      <c r="E2" s="47" t="s">
         <v>279</v>
       </c>
     </row>
@@ -19505,7 +19529,7 @@
       <c r="D3" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="E3" s="47" t="s">
         <v>282</v>
       </c>
     </row>
@@ -19522,7 +19546,7 @@
       <c r="D4" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="49" t="s">
+      <c r="E4" s="47" t="s">
         <v>306</v>
       </c>
     </row>
@@ -19539,7 +19563,7 @@
       <c r="D5" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="49" t="s">
+      <c r="E5" s="47" t="s">
         <v>306</v>
       </c>
     </row>
@@ -19556,7 +19580,7 @@
       <c r="D6" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="49" t="s">
+      <c r="E6" s="47" t="s">
         <v>289</v>
       </c>
     </row>
@@ -19573,7 +19597,7 @@
       <c r="D7" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="49" t="s">
+      <c r="E7" s="47" t="s">
         <v>307</v>
       </c>
       <c r="H7" s="34"/>
@@ -19581,7 +19605,7 @@
       <c r="J7" s="34"/>
       <c r="K7" s="34"/>
       <c r="L7" s="34"/>
-      <c r="M7" s="47"/>
+      <c r="M7" s="45"/>
       <c r="N7" s="34"/>
       <c r="O7" s="34"/>
     </row>
@@ -19598,7 +19622,7 @@
       <c r="D8" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E8" s="49" t="s">
+      <c r="E8" s="47" t="s">
         <v>308</v>
       </c>
       <c r="H8" s="34"/>
@@ -19606,7 +19630,7 @@
       <c r="J8" s="34"/>
       <c r="K8" s="34"/>
       <c r="L8" s="34"/>
-      <c r="M8" s="47"/>
+      <c r="M8" s="45"/>
       <c r="N8" s="34"/>
       <c r="O8" s="34"/>
     </row>
@@ -19623,7 +19647,7 @@
       <c r="D9" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="49" t="s">
+      <c r="E9" s="47" t="s">
         <v>309</v>
       </c>
       <c r="H9" s="34"/>
@@ -19631,7 +19655,7 @@
       <c r="J9" s="34"/>
       <c r="K9" s="34"/>
       <c r="L9" s="34"/>
-      <c r="M9" s="47"/>
+      <c r="M9" s="45"/>
       <c r="N9" s="34"/>
       <c r="O9" s="34"/>
     </row>
@@ -19648,7 +19672,7 @@
       <c r="D10" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E10" s="49" t="s">
+      <c r="E10" s="47" t="s">
         <v>297</v>
       </c>
       <c r="H10" s="34"/>
@@ -19656,7 +19680,7 @@
       <c r="J10" s="34"/>
       <c r="K10" s="34"/>
       <c r="L10" s="34"/>
-      <c r="M10" s="47"/>
+      <c r="M10" s="45"/>
       <c r="N10" s="34"/>
       <c r="O10" s="34"/>
     </row>
@@ -19673,7 +19697,7 @@
       <c r="D11" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E11" s="49" t="s">
+      <c r="E11" s="47" t="s">
         <v>310</v>
       </c>
       <c r="H11" s="34"/>
@@ -19681,7 +19705,7 @@
       <c r="J11" s="34"/>
       <c r="K11" s="34"/>
       <c r="L11" s="34"/>
-      <c r="M11" s="47"/>
+      <c r="M11" s="45"/>
       <c r="N11" s="34"/>
       <c r="O11" s="34"/>
     </row>
@@ -19698,7 +19722,7 @@
       <c r="D12" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="49" t="s">
+      <c r="E12" s="47" t="s">
         <v>302</v>
       </c>
       <c r="H12" s="34"/>
@@ -19706,7 +19730,7 @@
       <c r="J12" s="34"/>
       <c r="K12" s="34"/>
       <c r="L12" s="34"/>
-      <c r="M12" s="47"/>
+      <c r="M12" s="45"/>
       <c r="N12" s="34"/>
       <c r="O12" s="34"/>
     </row>
@@ -19723,7 +19747,7 @@
       <c r="D13" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="49" t="s">
+      <c r="E13" s="47" t="s">
         <v>311</v>
       </c>
       <c r="H13" s="34"/>
@@ -19731,7 +19755,7 @@
       <c r="J13" s="34"/>
       <c r="K13" s="34"/>
       <c r="L13" s="34"/>
-      <c r="M13" s="47"/>
+      <c r="M13" s="45"/>
       <c r="N13" s="34"/>
       <c r="O13" s="34"/>
     </row>
@@ -19748,7 +19772,7 @@
       <c r="D14" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E14" s="49">
+      <c r="E14" s="47">
         <v>43</v>
       </c>
       <c r="H14" s="34"/>
@@ -19756,7 +19780,7 @@
       <c r="J14" s="34"/>
       <c r="K14" s="34"/>
       <c r="L14" s="34"/>
-      <c r="M14" s="47"/>
+      <c r="M14" s="45"/>
       <c r="N14" s="34"/>
       <c r="O14" s="34"/>
     </row>
@@ -19773,7 +19797,7 @@
       <c r="D15" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E15" s="49">
+      <c r="E15" s="47">
         <v>60</v>
       </c>
       <c r="H15" s="34"/>
@@ -19781,7 +19805,7 @@
       <c r="J15" s="34"/>
       <c r="K15" s="34"/>
       <c r="L15" s="34"/>
-      <c r="M15" s="47"/>
+      <c r="M15" s="45"/>
       <c r="N15" s="34"/>
       <c r="O15" s="34"/>
     </row>
@@ -19798,7 +19822,7 @@
       <c r="D16" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="49" t="s">
+      <c r="E16" s="47" t="s">
         <v>312</v>
       </c>
       <c r="H16" s="34"/>
@@ -19806,7 +19830,7 @@
       <c r="J16" s="34"/>
       <c r="K16" s="34"/>
       <c r="L16" s="34"/>
-      <c r="M16" s="47"/>
+      <c r="M16" s="45"/>
       <c r="N16" s="34"/>
       <c r="O16" s="34"/>
     </row>
@@ -19823,7 +19847,7 @@
       <c r="D17" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="49" t="s">
+      <c r="E17" s="47" t="s">
         <v>313</v>
       </c>
       <c r="H17" s="34"/>
@@ -19831,7 +19855,7 @@
       <c r="J17" s="34"/>
       <c r="K17" s="34"/>
       <c r="L17" s="34"/>
-      <c r="M17" s="47"/>
+      <c r="M17" s="45"/>
       <c r="N17" s="34"/>
       <c r="O17" s="34"/>
     </row>
@@ -19848,7 +19872,7 @@
       <c r="D18" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E18" s="49" t="s">
+      <c r="E18" s="47" t="s">
         <v>314</v>
       </c>
       <c r="H18" s="34"/>
@@ -19856,7 +19880,7 @@
       <c r="J18" s="34"/>
       <c r="K18" s="34"/>
       <c r="L18" s="34"/>
-      <c r="M18" s="47"/>
+      <c r="M18" s="45"/>
       <c r="N18" s="34"/>
       <c r="O18" s="34"/>
     </row>
@@ -19864,7 +19888,7 @@
       <c r="A19" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="46" t="s">
         <v>96</v>
       </c>
       <c r="C19" s="11" t="s">
@@ -19873,7 +19897,7 @@
       <c r="D19" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="49" t="s">
+      <c r="E19" s="47" t="s">
         <v>315</v>
       </c>
       <c r="H19" s="34"/>
@@ -19881,7 +19905,7 @@
       <c r="J19" s="34"/>
       <c r="K19" s="34"/>
       <c r="L19" s="34"/>
-      <c r="M19" s="47"/>
+      <c r="M19" s="45"/>
       <c r="N19" s="34"/>
       <c r="O19" s="34"/>
     </row>
@@ -19898,12 +19922,12 @@
       <c r="D20" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="49" t="s">
+      <c r="E20" s="47" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="48" t="s">
+      <c r="A21" s="46" t="s">
         <v>99</v>
       </c>
       <c r="B21" s="11" t="s">
@@ -19915,13 +19939,18 @@
       <c r="D21" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="49"/>
+      <c r="E21" s="47" t="s">
+        <v>334</v>
+      </c>
+      <c r="F21" s="46" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="B22" s="48" t="s">
+      <c r="B22" s="46" t="s">
         <v>102</v>
       </c>
       <c r="C22" s="11" t="s">
@@ -19930,7 +19959,7 @@
       <c r="D22" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E22" s="49" t="s">
+      <c r="E22" s="47" t="s">
         <v>317</v>
       </c>
     </row>
@@ -19947,7 +19976,7 @@
       <c r="D23" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E23" s="49" t="s">
+      <c r="E23" s="47" t="s">
         <v>318</v>
       </c>
     </row>
@@ -19964,7 +19993,7 @@
       <c r="D24" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E24" s="49" t="s">
+      <c r="E24" s="47" t="s">
         <v>319</v>
       </c>
     </row>
@@ -19981,7 +20010,9 @@
       <c r="D25" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="49"/>
+      <c r="E25" s="47" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="15" t="s">
@@ -19996,7 +20027,12 @@
       <c r="D26" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="49"/>
+      <c r="E26" s="47" t="s">
+        <v>316</v>
+      </c>
+      <c r="F26" s="46" t="s">
+        <v>340</v>
+      </c>
     </row>
     <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="11" t="s">
@@ -20011,7 +20047,7 @@
       <c r="D27" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="49" t="s">
+      <c r="E27" s="47" t="s">
         <v>319</v>
       </c>
     </row>
@@ -20028,7 +20064,7 @@
       <c r="D28" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E28" s="49" t="s">
+      <c r="E28" s="47" t="s">
         <v>320</v>
       </c>
     </row>
@@ -20045,7 +20081,7 @@
       <c r="D29" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E29" s="49" t="s">
+      <c r="E29" s="47" t="s">
         <v>307</v>
       </c>
     </row>
@@ -20062,7 +20098,7 @@
       <c r="D30" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E30" s="49" t="s">
+      <c r="E30" s="47" t="s">
         <v>311</v>
       </c>
     </row>
@@ -20070,7 +20106,7 @@
       <c r="A31" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="B31" s="48" t="s">
+      <c r="B31" s="46" t="s">
         <v>120</v>
       </c>
       <c r="C31" s="11" t="s">
@@ -20079,7 +20115,7 @@
       <c r="D31" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E31" s="49" t="s">
+      <c r="E31" s="47" t="s">
         <v>321</v>
       </c>
     </row>
@@ -20096,11 +20132,11 @@
       <c r="D32" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E32" s="49" t="s">
+      <c r="E32" s="47" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="11" t="s">
         <v>123</v>
       </c>
@@ -20113,11 +20149,11 @@
       <c r="D33" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E33" s="49" t="s">
+      <c r="E33" s="47" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="11" t="s">
         <v>127</v>
       </c>
@@ -20130,11 +20166,11 @@
       <c r="D34" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E34" s="49" t="s">
+      <c r="E34" s="47" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="11" t="s">
         <v>129</v>
       </c>
@@ -20147,15 +20183,15 @@
       <c r="D35" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E35" s="49" t="s">
+      <c r="E35" s="47" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="B36" s="48" t="s">
+      <c r="B36" s="46" t="s">
         <v>132</v>
       </c>
       <c r="C36" s="11" t="s">
@@ -20164,11 +20200,11 @@
       <c r="D36" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E36" s="49" t="s">
+      <c r="E36" s="47" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="11" t="s">
         <v>133</v>
       </c>
@@ -20181,12 +20217,17 @@
       <c r="D37" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E37" s="49"/>
-      <c r="F37" s="11" t="s">
+      <c r="E37" s="47" t="s">
+        <v>326</v>
+      </c>
+      <c r="F37" s="46" t="s">
+        <v>338</v>
+      </c>
+      <c r="G37" s="46" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="11" t="s">
         <v>135</v>
       </c>
@@ -20199,11 +20240,11 @@
       <c r="D38" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E38" s="49" t="s">
+      <c r="E38" s="47" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="11" t="s">
         <v>137</v>
       </c>
@@ -20216,15 +20257,15 @@
       <c r="D39" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E39" s="49" t="s">
+      <c r="E39" s="47" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="B40" s="48" t="s">
+      <c r="B40" s="46" t="s">
         <v>140</v>
       </c>
       <c r="C40" s="11" t="s">
@@ -20233,11 +20274,11 @@
       <c r="D40" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E40" s="49" t="s">
+      <c r="E40" s="47" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="11" t="s">
         <v>141</v>
       </c>
@@ -20250,11 +20291,11 @@
       <c r="D41" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E41" s="49" t="s">
+      <c r="E41" s="47" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="11" t="s">
         <v>143</v>
       </c>
@@ -20267,11 +20308,11 @@
       <c r="D42" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E42" s="49" t="s">
+      <c r="E42" s="47" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="15" t="s">
         <v>145</v>
       </c>
@@ -20284,11 +20325,11 @@
       <c r="D43" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E43" s="49" t="s">
+      <c r="E43" s="47" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="11" t="s">
         <v>147</v>
       </c>
@@ -20301,9 +20342,14 @@
       <c r="D44" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E44" s="49"/>
-    </row>
-    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E44" s="47" t="s">
+        <v>336</v>
+      </c>
+      <c r="F44" s="46" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="11" t="s">
         <v>150</v>
       </c>
@@ -20316,11 +20362,11 @@
       <c r="D45" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E45" s="49" t="s">
+      <c r="E45" s="47" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="11" t="s">
         <v>268</v>
       </c>
@@ -20333,7 +20379,7 @@
       <c r="D46" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E46" s="49" t="s">
+      <c r="E46" s="47" t="s">
         <v>333</v>
       </c>
     </row>

</xml_diff>